<commit_message>
Elaboracao da planilha de estoque exemplo
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -5,36 +5,127 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\Gustavio\Exemplo git\teste-gustavio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuri_\Desktop\Gustavio\Teste-Exemplo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBE32C1-19F3-4515-A2FB-EA2067050575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFA7EAE-41C9-4731-A95D-EBAD84404E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tb-produtos" sheetId="1" r:id="rId1"/>
+    <sheet name="tb-fornecedor" sheetId="5" r:id="rId2"/>
+    <sheet name="tb-funcionarios" sheetId="6" r:id="rId3"/>
+    <sheet name="tb-entrada" sheetId="2" r:id="rId4"/>
+    <sheet name="tb-saida" sheetId="3" r:id="rId5"/>
+    <sheet name="rascunho" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>COCA-COLA 2L</t>
+  </si>
+  <si>
+    <t>fornecedor</t>
+  </si>
+  <si>
+    <t>COCA-COLA</t>
+  </si>
+  <si>
+    <t>id_produto</t>
+  </si>
+  <si>
+    <t>nome_produto</t>
+  </si>
+  <si>
+    <t>PASTEL</t>
+  </si>
+  <si>
+    <t>AGUA</t>
+  </si>
+  <si>
+    <t>quantidade</t>
+  </si>
+  <si>
+    <t>valor total</t>
+  </si>
+  <si>
+    <t>valor unitario</t>
+  </si>
+  <si>
+    <t>estoque</t>
+  </si>
+  <si>
+    <t>data atual</t>
+  </si>
+  <si>
+    <t>valor_unitário_venda</t>
+  </si>
+  <si>
+    <t>valor_total_venda</t>
+  </si>
+  <si>
+    <t>AMBEV</t>
+  </si>
+  <si>
+    <t>PETROPOLIS</t>
+  </si>
+  <si>
+    <t>Yuri</t>
+  </si>
+  <si>
+    <t>Alexandra</t>
+  </si>
+  <si>
+    <t>Gustavio</t>
+  </si>
+  <si>
+    <t>id_funcionario</t>
+  </si>
+  <si>
+    <t>nome_funcionario</t>
+  </si>
+  <si>
+    <t>Vendas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,16 +133,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -59,12 +184,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,18 +607,769 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="13.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4">
+        <f>SUMIFS('tb-entrada'!$F:$F,'tb-entrada'!$D:$D,'tb-produtos'!A2,'tb-entrada'!B:B,"&lt;=" &amp; 'tb-produtos'!F3)-SUMIFS('tb-saida'!$E:$E,'tb-saida'!$C:$C,'tb-produtos'!A2,'tb-saida'!$B:$B,"&lt;=" &amp; 'tb-produtos'!F3)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="16">
+        <v>45112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB61A2F5-D3C9-4737-A23D-131E4AE92C65}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A2009C-B61F-4EC7-AF12-DC39C89115C5}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC2595A-983A-488F-B21D-F192A3D48962}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>45108</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="str">
+        <f>VLOOKUP(D2,'tb-produtos'!A:B,2,FALSE)</f>
+        <v>COCA-COLA 2L</v>
+      </c>
+      <c r="F2" s="3">
+        <v>15</v>
+      </c>
+      <c r="G2" s="6">
+        <v>108</v>
+      </c>
+      <c r="H2" s="6">
+        <f>G2/F2</f>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C135C4AA-16AD-4DD9-9958-869524F78641}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>45111</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f>VLOOKUP(C2,'tb-produtos'!$A:$B,2,0)</f>
+        <v>COCA-COLA 2L</v>
+      </c>
+      <c r="E2" s="3">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6">
+        <f>F2*E2</f>
+        <v>48</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>VLOOKUP(H2,'tb-funcionarios'!A:B,2,0)</f>
+        <v>Alexandra</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>45112</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f>VLOOKUP(C3,'tb-produtos'!$A:$B,2,0)</f>
+        <v>COCA-COLA 2L</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6">
+        <f>F3*E3</f>
+        <v>24</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <f>VLOOKUP(H3,'tb-funcionarios'!A:B,2,0)</f>
+        <v>Gustavio</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9856B4F9-8F24-48DB-ADC1-5E4DB40146CF}">
+  <dimension ref="E3:I26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="5:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="23"/>
+    </row>
+    <row r="5" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E6" s="1"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E7" s="1"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E8" s="1"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E9" s="1"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E10" s="1"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E15" s="1"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E16" s="1"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E18" s="1"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E19" s="1"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E20" s="1"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E21" s="1"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E22" s="1"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E23" s="1"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E24" s="1"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E25" s="1"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E4:I4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>